<commit_message>
Bug Fix: Contact form and OTP generation
</commit_message>
<xml_diff>
--- a/private/contacts.xlsx
+++ b/private/contacts.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
   <si>
     <t>Name</t>
   </si>
@@ -131,6 +131,18 @@
   </si>
   <si>
     <t>27/3/2025, 2:43:36 pm</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>11/11/2025, 10:26:01 pm</t>
+  </si>
+  <si>
+    <t>Robert</t>
+  </si>
+  <si>
+    <t>11/11/2025, 10:54:36 pm</t>
   </si>
 </sst>
 </file>
@@ -507,7 +519,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E12"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -680,6 +692,40 @@
         <v>39</v>
       </c>
     </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
Fix: generate Excel in memory and upload to Supabase storage
</commit_message>
<xml_diff>
--- a/private/contacts.xlsx
+++ b/private/contacts.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
   <si>
     <t>Name</t>
   </si>
@@ -143,6 +143,12 @@
   </si>
   <si>
     <t>11/11/2025, 10:54:36 pm</t>
+  </si>
+  <si>
+    <t>ahmed</t>
+  </si>
+  <si>
+    <t>11/11/2025, 11:43:45 pm</t>
   </si>
 </sst>
 </file>
@@ -519,7 +525,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -726,6 +732,23 @@
         <v>43</v>
       </c>
     </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>